<commit_message>
✅ testing redis cache
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MTS5-3MCT-WAD\ResearchProject\research-project-3mct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{06B79568-40FA-4037-ADCD-D7D956853B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4D80AD-6DA5-4F8A-BA58-8C6D6196D00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="1230" yWindow="405" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Caching meetresultaten</t>
   </si>
@@ -42,12 +42,6 @@
     <t>Backend</t>
   </si>
   <si>
-    <t>Apollo Server</t>
-  </si>
-  <si>
-    <t>Data Size</t>
-  </si>
-  <si>
     <t>Redis Cache</t>
   </si>
   <si>
@@ -57,9 +51,6 @@
     <t>10 KB - 15 KB</t>
   </si>
   <si>
-    <t>ms</t>
-  </si>
-  <si>
     <t>Top Level Records</t>
   </si>
   <si>
@@ -69,14 +60,39 @@
     <t>Afhankelijk van het aantal records opgevraagd van de nested element, veranderen de tijden</t>
   </si>
   <si>
-    <t>100 KB - 15 KB</t>
+    <t>gemidd x sneller</t>
+  </si>
+  <si>
+    <t>100 KB - 115 KB</t>
+  </si>
+  <si>
+    <r>
+      <t>Response Size</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (in playground, niet 100% represatief met echte database data die gestored wordt in de cache)</t>
+    </r>
+  </si>
+  <si>
+    <t>500 KB - 511 KB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,8 +123,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +164,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -143,10 +186,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -156,8 +200,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Procent" xfId="1" builtinId="5"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -182,16 +234,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>266701</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>552451</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>120104</xdr:rowOff>
+      <xdr:rowOff>110579</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -214,7 +266,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9696451" y="819149"/>
+          <a:off x="15544801" y="809624"/>
           <a:ext cx="1362074" cy="2425155"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -226,16 +278,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>352426</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>133351</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>5082</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>395607</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
+      <xdr:rowOff>123826</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -258,7 +310,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11001376" y="838201"/>
+          <a:off x="16954501" y="828676"/>
           <a:ext cx="2091056" cy="704850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -567,27 +619,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -603,34 +657,36 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-      <c r="O3" t="s">
+      <c r="X3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="B4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="6"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" s="4">
         <v>20</v>
@@ -649,17 +705,23 @@
         <v>40</v>
       </c>
       <c r="H5" s="4">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
+      <c r="J5" s="4">
+        <v>2000</v>
+      </c>
+      <c r="K5" s="4">
+        <v>185</v>
+      </c>
+      <c r="L5" s="4">
+        <v>140</v>
+      </c>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
@@ -681,63 +743,112 @@
         <v>3</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
+      <c r="J6" s="4">
+        <v>1</v>
+      </c>
+      <c r="K6" s="4">
+        <v>2</v>
+      </c>
+      <c r="L6" s="4">
+        <v>3</v>
+      </c>
       <c r="M6" s="4"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="8">
         <v>11</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="8">
         <v>24</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="8">
         <v>80</v>
       </c>
-      <c r="F9">
+      <c r="E9" s="8"/>
+      <c r="F9" s="8">
         <v>25</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="8">
         <v>95</v>
       </c>
-      <c r="H9">
-        <v>6300</v>
-      </c>
+      <c r="H9" s="8">
+        <v>650</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8">
+        <v>100</v>
+      </c>
+      <c r="K9" s="8">
+        <v>430</v>
+      </c>
+      <c r="L9" s="8">
+        <v>2500</v>
+      </c>
+      <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>16</v>
-      </c>
-      <c r="D10">
-        <v>70</v>
-      </c>
-      <c r="F10">
-        <v>16</v>
-      </c>
-      <c r="G10">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>2</v>
+      </c>
+      <c r="B10" s="9">
+        <v>6</v>
+      </c>
+      <c r="C10" s="9">
+        <v>12</v>
+      </c>
+      <c r="D10" s="9">
+        <v>24</v>
+      </c>
+      <c r="E10" s="10">
+        <f>SUM(B9:D9)/SUM(B10:D10)</f>
+        <v>2.7380952380952381</v>
+      </c>
+      <c r="F10" s="9">
+        <v>18</v>
+      </c>
+      <c r="G10" s="9">
+        <v>25</v>
+      </c>
+      <c r="H10" s="9">
+        <v>50</v>
+      </c>
+      <c r="I10" s="11">
+        <f>SUM(F9:H9)/SUM(F10:H10)</f>
+        <v>8.279569892473118</v>
+      </c>
+      <c r="J10" s="9">
+        <v>63</v>
+      </c>
+      <c r="K10" s="9">
+        <v>65</v>
+      </c>
+      <c r="L10" s="9">
+        <v>200</v>
+      </c>
+      <c r="M10" s="11">
+        <f>SUM(J9:L9)/SUM(J10:L10)</f>
+        <v>9.2378048780487809</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="F4:H4"/>
+    <mergeCell ref="J4:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
✅ Ready for client side testing
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MTS5-3MCT-WAD\ResearchProject\research-project-3mct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C4DB0D-74DB-4CF4-A6A4-28A3DCA8DCAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E596BC9-499C-4D89-979F-E45608DBB9F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Meetingen" sheetId="1" r:id="rId1"/>
-    <sheet name="n sneller data grote" sheetId="2" r:id="rId2"/>
-    <sheet name="n sneller nesting" sheetId="3" r:id="rId3"/>
+    <sheet name="Meetingen" sheetId="4" r:id="rId1"/>
+    <sheet name="Meetingen frontend &amp; backend" sheetId="5" r:id="rId2"/>
+    <sheet name="n sneller data grote" sheetId="2" r:id="rId3"/>
+    <sheet name="n sneller nesting" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="26">
   <si>
     <t>Caching meetresultaten</t>
   </si>
@@ -57,9 +58,6 @@
   </si>
   <si>
     <t>Nesting Level</t>
-  </si>
-  <si>
-    <t>Afhankelijk van het aantal records opgevraagd van de nested element, veranderen de tijden</t>
   </si>
   <si>
     <t>gemidd x sneller</t>
@@ -103,6 +101,33 @@
   </si>
   <si>
     <t>4 levels</t>
+  </si>
+  <si>
+    <t>Frontend data size</t>
+  </si>
+  <si>
+    <t>Frontend</t>
+  </si>
+  <si>
+    <t>4,18 kB</t>
+  </si>
+  <si>
+    <t>51,51 kB</t>
+  </si>
+  <si>
+    <t>1,11 kB</t>
+  </si>
+  <si>
+    <t>6,12 kB</t>
+  </si>
+  <si>
+    <t>user 1</t>
+  </si>
+  <si>
+    <t>post 4</t>
+  </si>
+  <si>
+    <t>gemidd x sneller dan zonder cache</t>
   </si>
 </sst>
 </file>
@@ -159,7 +184,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,6 +221,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -210,7 +247,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -228,7 +265,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Procent" xfId="1" builtinId="5"/>
@@ -1967,99 +2009,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>552451</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>110579</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Afbeelding 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9A5203C-9B68-4AAB-BF9C-6382C074788C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15544801" y="809624"/>
-          <a:ext cx="1362074" cy="2425155"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>133351</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>395607</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Afbeelding 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D683A26C-7377-4BAB-80CE-2ECA5D0213BE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="16954501" y="828676"/>
-          <a:ext cx="2091056" cy="704850"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -2099,7 +2048,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2436,30 +2385,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B62396A-1EEF-4886-A0B4-50F17905706F}">
+  <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="15.85546875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2479,42 +2419,39 @@
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
-      <c r="X3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11" t="s">
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6" t="s">
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -2557,7 +2494,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -2600,24 +2537,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>3</v>
       </c>
@@ -2661,7 +2598,7 @@
       </c>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>2</v>
       </c>
@@ -2720,26 +2657,257 @@
         <v>8.5714285714285712</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="Q11" s="13"/>
-    </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
     <mergeCell ref="J4:M4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="B4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A49B06-8EDD-4703-89E7-71FF6DEBDE86}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
+        <v>50</v>
+      </c>
+      <c r="C5" s="4">
+        <v>50</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="14">
+        <v>122</v>
+      </c>
+      <c r="C10" s="14">
+        <v>450</v>
+      </c>
+      <c r="D10" s="14">
+        <v>40</v>
+      </c>
+      <c r="E10" s="14">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="15">
+        <v>20</v>
+      </c>
+      <c r="C11" s="15">
+        <v>370</v>
+      </c>
+      <c r="D11" s="15">
+        <v>28</v>
+      </c>
+      <c r="E11" s="15">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f>AVERAGE(B10:B11)</f>
+        <v>71</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:E12" si="0">AVERAGE(C10:C11)</f>
+        <v>410</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="14">
+        <v>62</v>
+      </c>
+      <c r="C14" s="14">
+        <v>90</v>
+      </c>
+      <c r="D14" s="14">
+        <v>23</v>
+      </c>
+      <c r="E14" s="14">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="15">
+        <v>10</v>
+      </c>
+      <c r="C15" s="15">
+        <v>25</v>
+      </c>
+      <c r="D15" s="15">
+        <v>12</v>
+      </c>
+      <c r="E15" s="15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f>AVERAGE(B14:B15)</f>
+        <v>36</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:E16" si="1">AVERAGE(C14:C15)</f>
+        <v>57.5</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>17.5</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="12">
+        <f>B12/B16</f>
+        <v>1.9722222222222223</v>
+      </c>
+      <c r="C17" s="12">
+        <f>C12/C16</f>
+        <v>7.1304347826086953</v>
+      </c>
+      <c r="D17" s="12">
+        <f>D12/D16</f>
+        <v>1.9428571428571428</v>
+      </c>
+      <c r="E17" s="12">
+        <f>E12/E16</f>
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C6A869-BC33-4152-8637-9185423EF725}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q30"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2756,16 +2924,16 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2794,7 +2962,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53CE187-2852-45DF-91A3-78FFA61430C8}">
   <dimension ref="A1:R30"/>
   <sheetViews>
@@ -2835,33 +3003,33 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -2952,19 +3120,19 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -3235,16 +3403,16 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
         <v>14</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>15</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>16</v>
-      </c>
-      <c r="E29" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
⚙️ Init apollo client
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MTS5-3MCT-WAD\ResearchProject\research-project-3mct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E596BC9-499C-4D89-979F-E45608DBB9F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6DD631-4B94-4CFF-8874-DE42B8BA111D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1230" yWindow="405" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetingen" sheetId="4" r:id="rId1"/>
@@ -265,12 +265,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Procent" xfId="1" builtinId="5"/>
@@ -2424,24 +2424,24 @@
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13" t="s">
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
       <c r="N4" s="11"/>
       <c r="O4" s="11" t="s">
         <v>11</v>
@@ -2672,7 +2672,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2707,16 +2707,16 @@
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="15" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2764,36 +2764,36 @@
       <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="13">
         <v>122</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="13">
         <v>450</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="13">
         <v>40</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="13">
         <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="14">
         <v>20</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="14">
         <v>370</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <v>28</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="14">
         <v>210</v>
       </c>
     </row>
@@ -2825,36 +2825,36 @@
       <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="13">
         <v>62</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="13">
         <v>90</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="13">
         <v>23</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="13">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="14">
         <v>10</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="14">
         <v>25</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="14">
         <v>12</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="14">
         <v>15</v>
       </c>
     </row>
@@ -3005,24 +3005,24 @@
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13" t="s">
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
⚙️ Measure mount data times
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MTS5-3MCT-WAD\ResearchProject\research-project-3mct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6DD631-4B94-4CFF-8874-DE42B8BA111D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A257101-D0B2-4510-99E1-CA8420F1D9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="405" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetingen" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="31">
   <si>
     <t>Caching meetresultaten</t>
   </si>
@@ -115,19 +115,34 @@
     <t>51,51 kB</t>
   </si>
   <si>
-    <t>1,11 kB</t>
-  </si>
-  <si>
     <t>6,12 kB</t>
   </si>
   <si>
     <t>user 1</t>
   </si>
   <si>
-    <t>post 4</t>
+    <t>posts</t>
   </si>
   <si>
-    <t>gemidd x sneller dan zonder cache</t>
+    <t>users</t>
+  </si>
+  <si>
+    <t>post 12</t>
+  </si>
+  <si>
+    <t>2,47 kB</t>
+  </si>
+  <si>
+    <t>Netwerk gemidd x sneller dan zonder cache</t>
+  </si>
+  <si>
+    <t>mount tot data inladen x sneller dan zonder cache</t>
+  </si>
+  <si>
+    <t>mount tot inladen data</t>
+  </si>
+  <si>
+    <t>Apollo client cache</t>
   </si>
 </sst>
 </file>
@@ -184,7 +199,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,6 +248,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -247,7 +268,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -271,6 +292,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Procent" xfId="1" builtinId="5"/>
@@ -2669,15 +2692,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A49B06-8EDD-4703-89E7-71FF6DEBDE86}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2687,11 +2710,17 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2714,10 +2743,10 @@
         <v>20</v>
       </c>
       <c r="D4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>21</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2768,16 +2797,16 @@
         <v>18</v>
       </c>
       <c r="B10" s="13">
-        <v>122</v>
+        <v>19</v>
       </c>
       <c r="C10" s="13">
-        <v>450</v>
+        <v>332</v>
       </c>
       <c r="D10" s="13">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E10" s="13">
-        <v>230</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2785,116 +2814,214 @@
         <v>1</v>
       </c>
       <c r="B11" s="14">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C11" s="14">
-        <v>370</v>
+        <v>330</v>
       </c>
       <c r="D11" s="14">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E11" s="14">
-        <v>210</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12">
         <f>AVERAGE(B10:B11)</f>
-        <v>71</v>
+        <v>17.5</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12:E12" si="0">AVERAGE(C10:C11)</f>
-        <v>410</v>
+        <f t="shared" ref="C12:D12" si="0">AVERAGE(C10:C11)</f>
+        <v>331</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>36.5</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
-        <v>220</v>
+        <f>AVERAGE(E10:E11)</f>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="18">
+        <v>121</v>
+      </c>
+      <c r="C13" s="18">
+        <v>520</v>
+      </c>
+      <c r="D13" s="18">
+        <v>125</v>
+      </c>
+      <c r="E13" s="18">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="9"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="13">
-        <v>62</v>
-      </c>
-      <c r="C14" s="13">
-        <v>90</v>
-      </c>
-      <c r="D14" s="13">
-        <v>23</v>
-      </c>
-      <c r="E14" s="13">
+      <c r="B17" s="13">
+        <v>19</v>
+      </c>
+      <c r="C17" s="13">
+        <v>38</v>
+      </c>
+      <c r="D17" s="13">
+        <v>16</v>
+      </c>
+      <c r="E17" s="13">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="14">
+        <v>15</v>
+      </c>
+      <c r="C18" s="14">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="14">
-        <v>10</v>
-      </c>
-      <c r="C15" s="14">
-        <v>25</v>
-      </c>
-      <c r="D15" s="14">
-        <v>12</v>
-      </c>
-      <c r="E15" s="14">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <f>AVERAGE(B14:B15)</f>
-        <v>36</v>
-      </c>
-      <c r="C16">
-        <f t="shared" ref="C16:E16" si="1">AVERAGE(C14:C15)</f>
-        <v>57.5</v>
-      </c>
-      <c r="D16">
+      <c r="D18" s="14">
+        <v>13</v>
+      </c>
+      <c r="E18" s="14">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f>AVERAGE(B17:B18)</f>
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19:E19" si="1">AVERAGE(C17:C18)</f>
+        <v>36.5</v>
+      </c>
+      <c r="D19">
         <f t="shared" si="1"/>
-        <v>17.5</v>
-      </c>
-      <c r="E16">
+        <v>14.5</v>
+      </c>
+      <c r="E19">
         <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="12">
-        <f>B12/B16</f>
-        <v>1.9722222222222223</v>
-      </c>
-      <c r="C17" s="12">
-        <f>C12/C16</f>
-        <v>7.1304347826086953</v>
-      </c>
-      <c r="D17" s="12">
-        <f>D12/D16</f>
-        <v>1.9428571428571428</v>
-      </c>
-      <c r="E17" s="12">
-        <f>E12/E16</f>
-        <v>8.8000000000000007</v>
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="18">
+        <v>119</v>
+      </c>
+      <c r="C20" s="18">
+        <v>289</v>
+      </c>
+      <c r="D20" s="18">
+        <v>102</v>
+      </c>
+      <c r="E20" s="18">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="13">
+        <v>19</v>
+      </c>
+      <c r="C24" s="13">
+        <v>38</v>
+      </c>
+      <c r="D24" s="13">
+        <v>16</v>
+      </c>
+      <c r="E24" s="13">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="18">
+        <v>119</v>
+      </c>
+      <c r="C26" s="18">
+        <v>289</v>
+      </c>
+      <c r="D26" s="18">
+        <v>102</v>
+      </c>
+      <c r="E26" s="18">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="17">
+        <f>B13/B20</f>
+        <v>1.0168067226890756</v>
+      </c>
+      <c r="C33" s="17">
+        <f>C13/C20</f>
+        <v>1.7993079584775087</v>
+      </c>
+      <c r="D33" s="17">
+        <f>D13/D20</f>
+        <v>1.2254901960784315</v>
+      </c>
+      <c r="E33" s="17">
+        <f>E13/E20</f>
+        <v>1.5564516129032258</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="12">
+        <f>B12/B19</f>
+        <v>1.0294117647058822</v>
+      </c>
+      <c r="C34" s="12">
+        <f>C12/C19</f>
+        <v>9.0684931506849313</v>
+      </c>
+      <c r="D34" s="12">
+        <f>D12/D19</f>
+        <v>2.5172413793103448</v>
+      </c>
+      <c r="E34" s="12">
+        <f>E12/E19</f>
+        <v>4.3555555555555552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
⚙️ Apollo client cache works
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MTS5-3MCT-WAD\ResearchProject\research-project-3mct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A257101-D0B2-4510-99E1-CA8420F1D9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656A75E1-DDF2-47C6-8E4C-D7220256B015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="735" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetingen" sheetId="4" r:id="rId1"/>
@@ -289,11 +289,11 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Procent" xfId="1" builtinId="5"/>
@@ -2447,24 +2447,24 @@
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16" t="s">
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
       <c r="N4" s="11"/>
       <c r="O4" s="11" t="s">
         <v>11</v>
@@ -2694,8 +2694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A49B06-8EDD-4703-89E7-71FF6DEBDE86}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2845,19 +2845,19 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="17">
         <v>121</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="17">
         <v>520</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="17">
         <v>125</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="17">
         <v>193</v>
       </c>
     </row>
@@ -2923,19 +2923,19 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B20" s="17">
         <v>119</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="17">
         <v>289</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="17">
         <v>102</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="17">
         <v>124</v>
       </c>
     </row>
@@ -2966,19 +2966,19 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="18">
-        <v>119</v>
-      </c>
-      <c r="C26" s="18">
-        <v>289</v>
-      </c>
-      <c r="D26" s="18">
+      <c r="B26" s="17">
+        <v>53</v>
+      </c>
+      <c r="C26" s="17">
+        <v>124</v>
+      </c>
+      <c r="D26" s="17">
         <v>102</v>
       </c>
-      <c r="E26" s="18">
+      <c r="E26" s="17">
         <v>124</v>
       </c>
     </row>
@@ -2986,19 +2986,19 @@
       <c r="A33" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="17">
+      <c r="B33" s="16">
         <f>B13/B20</f>
         <v>1.0168067226890756</v>
       </c>
-      <c r="C33" s="17">
+      <c r="C33" s="16">
         <f>C13/C20</f>
         <v>1.7993079584775087</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="16">
         <f>D13/D20</f>
         <v>1.2254901960784315</v>
       </c>
-      <c r="E33" s="17">
+      <c r="E33" s="16">
         <f>E13/E20</f>
         <v>1.5564516129032258</v>
       </c>
@@ -3132,24 +3132,24 @@
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16" t="s">
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
☑️ Measurements up to data na mac tests
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MTS5-3MCT-WAD\ResearchProject\research-project-3mct\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nielsonderbeke/Desktop/3MCT-WAD/research-project/research-project-3mct/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656A75E1-DDF2-47C6-8E4C-D7220256B015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6CC1B3-9186-3A4E-8CEB-2FA721551738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="735" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="17280" windowHeight="19860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetingen" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="32">
   <si>
     <t>Caching meetresultaten</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Apollo client cache</t>
+  </si>
+  <si>
+    <t>content length</t>
   </si>
 </sst>
 </file>
@@ -296,8 +299,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Procent" xfId="1" builtinId="5"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -320,7 +323,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -382,7 +385,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-BE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -513,7 +516,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-BE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="492751472"/>
@@ -572,7 +575,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-BE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="581892496"/>
@@ -620,7 +623,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-BE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -634,7 +637,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -701,7 +704,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-BE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -826,7 +829,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-BE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="581874256"/>
@@ -885,7 +888,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-BE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="581872016"/>
@@ -933,7 +936,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-BE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2113,7 +2116,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2415,14 +2418,14 @@
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2443,7 +2446,7 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -2474,7 +2477,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -2517,7 +2520,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -2560,7 +2563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
         <v>7</v>
       </c>
@@ -2577,7 +2580,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>3</v>
       </c>
@@ -2621,7 +2624,7 @@
       </c>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>2</v>
       </c>
@@ -2695,21 +2698,21 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>24</v>
       </c>
@@ -2723,7 +2726,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2732,248 +2735,242 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="3">
+        <v>4302</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C5" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D5" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E5" s="15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B6" s="4">
         <v>50</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C6" s="4">
         <v>50</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D6" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E6" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C7" s="4">
         <v>2</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D7" s="4">
         <v>3</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E7" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="13">
-        <v>19</v>
-      </c>
-      <c r="C10" s="13">
-        <v>332</v>
-      </c>
-      <c r="D10" s="13">
-        <v>38</v>
-      </c>
-      <c r="E10" s="13">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="B11" s="13">
+        <v>32</v>
+      </c>
+      <c r="C11" s="13">
+        <v>185</v>
+      </c>
+      <c r="D11" s="13">
+        <v>45</v>
+      </c>
+      <c r="E11" s="13">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="14">
-        <v>16</v>
-      </c>
-      <c r="C11" s="14">
-        <v>330</v>
-      </c>
-      <c r="D11" s="14">
-        <v>35</v>
-      </c>
-      <c r="E11" s="14">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <f>AVERAGE(B10:B11)</f>
-        <v>17.5</v>
-      </c>
-      <c r="C12">
-        <f t="shared" ref="C12:D12" si="0">AVERAGE(C10:C11)</f>
-        <v>331</v>
-      </c>
-      <c r="D12">
+      <c r="B12" s="14">
+        <v>30</v>
+      </c>
+      <c r="C12" s="14">
+        <v>184</v>
+      </c>
+      <c r="D12" s="14">
+        <v>41</v>
+      </c>
+      <c r="E12" s="14">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <f>AVERAGE(B11:B12)</f>
+        <v>31</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:D13" si="0">AVERAGE(C11:C12)</f>
+        <v>184.5</v>
+      </c>
+      <c r="D13">
         <f t="shared" si="0"/>
-        <v>36.5</v>
-      </c>
-      <c r="E12">
-        <f>AVERAGE(E10:E11)</f>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13">
+        <f>AVERAGE(E11:E12)</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="17">
-        <v>121</v>
-      </c>
-      <c r="C13" s="17">
-        <v>520</v>
-      </c>
-      <c r="D13" s="17">
-        <v>125</v>
-      </c>
-      <c r="E13" s="17">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="B14" s="17">
+        <v>57</v>
+      </c>
+      <c r="C14" s="17">
+        <v>255</v>
+      </c>
+      <c r="D14" s="17">
+        <v>82</v>
+      </c>
+      <c r="E14" s="17">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="13">
-        <v>19</v>
-      </c>
-      <c r="C17" s="13">
-        <v>38</v>
-      </c>
-      <c r="D17" s="13">
-        <v>16</v>
-      </c>
-      <c r="E17" s="13">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="B18" s="13">
+        <v>22</v>
+      </c>
+      <c r="C18" s="13">
+        <v>31</v>
+      </c>
+      <c r="D18" s="13">
+        <v>27</v>
+      </c>
+      <c r="E18" s="13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="14">
-        <v>15</v>
-      </c>
-      <c r="C18" s="14">
-        <v>35</v>
-      </c>
-      <c r="D18" s="14">
-        <v>13</v>
-      </c>
-      <c r="E18" s="14">
+      <c r="B19" s="14">
+        <v>20</v>
+      </c>
+      <c r="C19" s="14">
+        <v>29</v>
+      </c>
+      <c r="D19" s="14">
+        <v>26</v>
+      </c>
+      <c r="E19" s="14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <f>AVERAGE(B18:B19)</f>
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <f>AVERAGE(B17:B18)</f>
-        <v>17</v>
-      </c>
-      <c r="C19">
-        <f t="shared" ref="C19:E19" si="1">AVERAGE(C17:C18)</f>
-        <v>36.5</v>
-      </c>
-      <c r="D19">
+      <c r="C20">
+        <f t="shared" ref="C20:E20" si="1">AVERAGE(C18:C19)</f>
+        <v>30</v>
+      </c>
+      <c r="D20">
         <f t="shared" si="1"/>
-        <v>14.5</v>
-      </c>
-      <c r="E19">
+        <v>26.5</v>
+      </c>
+      <c r="E20">
         <f t="shared" si="1"/>
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="17">
-        <v>119</v>
-      </c>
-      <c r="C20" s="17">
-        <v>289</v>
-      </c>
-      <c r="D20" s="17">
-        <v>102</v>
-      </c>
-      <c r="E20" s="17">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="B21" s="17">
+        <v>52</v>
+      </c>
+      <c r="C21" s="17">
+        <v>69</v>
+      </c>
+      <c r="D21" s="17">
+        <v>63</v>
+      </c>
+      <c r="E21" s="17">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="9"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="13">
-        <v>19</v>
-      </c>
-      <c r="C24" s="13">
-        <v>38</v>
-      </c>
-      <c r="D24" s="13">
-        <v>16</v>
-      </c>
-      <c r="E24" s="13">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="17">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C26" s="17">
-        <v>124</v>
+        <v>77</v>
       </c>
       <c r="D26" s="17">
         <v>102</v>
@@ -2982,46 +2979,46 @@
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>28</v>
       </c>
       <c r="B33" s="16">
-        <f>B13/B20</f>
-        <v>1.0168067226890756</v>
+        <f>B14/B21</f>
+        <v>1.0961538461538463</v>
       </c>
       <c r="C33" s="16">
-        <f>C13/C20</f>
-        <v>1.7993079584775087</v>
+        <f>C14/C21</f>
+        <v>3.6956521739130435</v>
       </c>
       <c r="D33" s="16">
-        <f>D13/D20</f>
-        <v>1.2254901960784315</v>
+        <f>D14/D21</f>
+        <v>1.3015873015873016</v>
       </c>
       <c r="E33" s="16">
-        <f>E13/E20</f>
-        <v>1.5564516129032258</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <f>E14/E21</f>
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>27</v>
       </c>
       <c r="B34" s="12">
-        <f>B12/B19</f>
-        <v>1.0294117647058822</v>
+        <f>B13/B20</f>
+        <v>1.4761904761904763</v>
       </c>
       <c r="C34" s="12">
-        <f>C12/C19</f>
-        <v>9.0684931506849313</v>
+        <f>C13/C20</f>
+        <v>6.15</v>
       </c>
       <c r="D34" s="12">
-        <f>D12/D19</f>
-        <v>2.5172413793103448</v>
+        <f>D13/D20</f>
+        <v>1.6226415094339623</v>
       </c>
       <c r="E34" s="12">
-        <f>E12/E19</f>
-        <v>4.3555555555555552</v>
+        <f>E13/E20</f>
+        <v>2.193548387096774</v>
       </c>
     </row>
   </sheetData>
@@ -3037,16 +3034,16 @@
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -3063,7 +3060,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -3097,17 +3094,17 @@
       <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -3128,7 +3125,7 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -3159,7 +3156,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -3202,7 +3199,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -3245,7 +3242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
         <v>7</v>
       </c>
@@ -3262,7 +3259,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>3</v>
       </c>
@@ -3306,7 +3303,7 @@
       </c>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>2</v>
       </c>
@@ -3365,7 +3362,7 @@
         <v>8.5714285714285712</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>6</v>
       </c>
@@ -3403,7 +3400,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>3</v>
       </c>
@@ -3441,7 +3438,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>2</v>
       </c>
@@ -3479,7 +3476,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B26" s="12">
         <f>B24/B25</f>
         <v>1.8333333333333333</v>
@@ -3525,7 +3522,7 @@
         <v>8.5714285714285712</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>6</v>
       </c>
@@ -3542,7 +3539,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
☑️ Measure apollo client details pages
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nielsonderbeke/Desktop/3MCT-WAD/research-project/research-project-3mct/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6CC1B3-9186-3A4E-8CEB-2FA721551738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B83C67-D8F1-6846-8FFC-BA7235A305E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="17280" windowHeight="19860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2698,7 +2698,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2973,10 +2973,10 @@
         <v>77</v>
       </c>
       <c r="D26" s="17">
-        <v>102</v>
+        <v>16</v>
       </c>
       <c r="E26" s="17">
-        <v>124</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
☑️ we are getting somewhere http caching
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nielsonderbeke/Desktop/3MCT-WAD/research-project/research-project-3mct/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B83C67-D8F1-6846-8FFC-BA7235A305E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1DFDFA-FAC9-424F-8423-81F145999B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="17280" windowHeight="19860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="17280" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetingen" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="33">
   <si>
     <t>Caching meetresultaten</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>content length</t>
+  </si>
+  <si>
+    <t>Apollo client - persisted queries - without cdn - own server memory cache</t>
   </si>
 </sst>
 </file>
@@ -2695,10 +2698,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A49B06-8EDD-4703-89E7-71FF6DEBDE86}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2962,61 +2965,142 @@
       <c r="D24" s="8"/>
       <c r="E24" s="9"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="17">
+      <c r="B25" s="17">
         <v>41</v>
       </c>
-      <c r="C26" s="17">
+      <c r="C25" s="17">
         <v>77</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D25" s="17">
         <v>16</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E25" s="17">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="13">
+        <v>35</v>
+      </c>
+      <c r="C29" s="13">
+        <f>C30+1.5</f>
+        <v>182.5</v>
+      </c>
+      <c r="D29" s="13">
+        <f t="shared" ref="D29:E29" si="2">D30+1.5</f>
+        <v>36.5</v>
+      </c>
+      <c r="E29" s="13">
+        <f t="shared" si="2"/>
+        <v>56.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="14">
+        <v>33</v>
+      </c>
+      <c r="C30" s="14">
+        <v>181</v>
+      </c>
+      <c r="D30" s="14">
+        <v>35</v>
+      </c>
+      <c r="E30" s="14">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <f>AVERAGE(B29:B30)</f>
+        <v>34</v>
+      </c>
+      <c r="C31">
+        <f t="shared" ref="C31:E31" si="3">AVERAGE(C29:C30)</f>
+        <v>181.75</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="3"/>
+        <v>35.75</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="3"/>
+        <v>55.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="17">
+        <v>56</v>
+      </c>
+      <c r="C32" s="17">
+        <v>216</v>
+      </c>
+      <c r="D32" s="17">
+        <v>77</v>
+      </c>
+      <c r="E32" s="17">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="16">
+      <c r="B44" s="16">
         <f>B14/B21</f>
         <v>1.0961538461538463</v>
       </c>
-      <c r="C33" s="16">
+      <c r="C44" s="16">
         <f>C14/C21</f>
         <v>3.6956521739130435</v>
       </c>
-      <c r="D33" s="16">
+      <c r="D44" s="16">
         <f>D14/D21</f>
         <v>1.3015873015873016</v>
       </c>
-      <c r="E33" s="16">
+      <c r="E44" s="16">
         <f>E14/E21</f>
         <v>1.44</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="12">
+      <c r="B45" s="12">
         <f>B13/B20</f>
         <v>1.4761904761904763</v>
       </c>
-      <c r="C34" s="12">
+      <c r="C45" s="12">
         <f>C13/C20</f>
         <v>6.15</v>
       </c>
-      <c r="D34" s="12">
+      <c r="D45" s="12">
         <f>D13/D20</f>
         <v>1.6226415094339623</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E45" s="12">
         <f>E13/E20</f>
         <v>2.193548387096774</v>
       </c>

</xml_diff>

<commit_message>
☑️ Measurements HTTP caching
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nielsonderbeke/Desktop/3MCT-WAD/research-project/research-project-3mct/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1DFDFA-FAC9-424F-8423-81F145999B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D0EB19-719A-8740-AB65-EFE4188449CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="17280" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="53760" yWindow="500" windowWidth="19200" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetingen" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="32">
   <si>
     <t>Caching meetresultaten</t>
   </si>
@@ -133,22 +133,19 @@
     <t>2,47 kB</t>
   </si>
   <si>
-    <t>Netwerk gemidd x sneller dan zonder cache</t>
-  </si>
-  <si>
-    <t>mount tot data inladen x sneller dan zonder cache</t>
-  </si>
-  <si>
     <t>mount tot inladen data</t>
   </si>
   <si>
     <t>Apollo client cache</t>
   </si>
   <si>
-    <t>content length</t>
+    <t>Apollo client - persisted queries - without cdn - own server memory cache</t>
   </si>
   <si>
-    <t>Apollo client - persisted queries - without cdn - own server memory cache</t>
+    <t>Apollo client - persisted queries - without cdn - own server memory cache - HTTP CACHE</t>
+  </si>
+  <si>
+    <t>total ms</t>
   </si>
 </sst>
 </file>
@@ -205,7 +202,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,6 +257,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -274,7 +295,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -295,11 +316,19 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2453,24 +2482,24 @@
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18" t="s">
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
       <c r="N4" s="11"/>
       <c r="O4" s="11" t="s">
         <v>11</v>
@@ -2698,10 +2727,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A49B06-8EDD-4703-89E7-71FF6DEBDE86}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2710,12 +2739,12 @@
     <col min="2" max="5" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>24</v>
       </c>
@@ -2728,8 +2757,11 @@
       <c r="E2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2738,371 +2770,365 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
+        <v>50</v>
+      </c>
+      <c r="C5" s="4">
+        <v>50</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="13">
+        <v>32</v>
+      </c>
+      <c r="C10" s="13">
+        <v>185</v>
+      </c>
+      <c r="D10" s="13">
+        <v>45</v>
+      </c>
+      <c r="E10" s="13">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="14">
+        <v>30</v>
+      </c>
+      <c r="C11" s="14">
+        <v>184</v>
+      </c>
+      <c r="D11" s="14">
+        <v>41</v>
+      </c>
+      <c r="E11" s="14">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <f>AVERAGE(B10:B11)</f>
         <v>31</v>
       </c>
-      <c r="B4" s="3">
-        <v>4302</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4">
-        <v>50</v>
-      </c>
-      <c r="C6" s="4">
-        <v>50</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4">
-        <v>2</v>
-      </c>
-      <c r="D7" s="4">
-        <v>3</v>
-      </c>
-      <c r="E7" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="13">
-        <v>32</v>
-      </c>
-      <c r="C11" s="13">
-        <v>185</v>
-      </c>
-      <c r="D11" s="13">
-        <v>45</v>
-      </c>
-      <c r="E11" s="13">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="14">
-        <v>30</v>
-      </c>
-      <c r="C12" s="14">
-        <v>184</v>
-      </c>
-      <c r="D12" s="14">
-        <v>41</v>
-      </c>
-      <c r="E12" s="14">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13">
-        <f>AVERAGE(B11:B12)</f>
-        <v>31</v>
-      </c>
-      <c r="C13">
-        <f t="shared" ref="C13:D13" si="0">AVERAGE(C11:C12)</f>
+      <c r="C12">
+        <f t="shared" ref="C12:D12" si="0">AVERAGE(C10:C11)</f>
         <v>184.5</v>
       </c>
-      <c r="D13">
+      <c r="D12">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="E13">
-        <f>AVERAGE(E11:E12)</f>
+      <c r="E12">
+        <f>AVERAGE(E10:E11)</f>
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="16">
+        <v>57</v>
+      </c>
+      <c r="C13" s="16">
+        <v>255</v>
+      </c>
+      <c r="D13" s="16">
+        <v>82</v>
+      </c>
+      <c r="E13" s="16">
+        <v>108</v>
+      </c>
+      <c r="F13" s="16">
+        <f>SUM(B13:E13)</f>
+        <v>502</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="26"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="13">
+        <v>22</v>
+      </c>
+      <c r="C17" s="13">
+        <v>31</v>
+      </c>
+      <c r="D17" s="13">
+        <v>27</v>
+      </c>
+      <c r="E17" s="13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="14">
+        <v>20</v>
+      </c>
+      <c r="C18" s="14">
         <v>29</v>
       </c>
-      <c r="B14" s="17">
-        <v>57</v>
-      </c>
-      <c r="C14" s="17">
-        <v>255</v>
-      </c>
-      <c r="D14" s="17">
-        <v>82</v>
-      </c>
-      <c r="E14" s="17">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="9"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="13">
-        <v>22</v>
-      </c>
-      <c r="C18" s="13">
-        <v>31</v>
-      </c>
-      <c r="D18" s="13">
-        <v>27</v>
-      </c>
-      <c r="E18" s="13">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="14">
-        <v>20</v>
-      </c>
-      <c r="C19" s="14">
-        <v>29</v>
-      </c>
-      <c r="D19" s="14">
+      <c r="D18" s="14">
         <v>26</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E18" s="14">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B20">
-        <f>AVERAGE(B18:B19)</f>
+      <c r="I18" s="22"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <f>AVERAGE(B17:B18)</f>
         <v>21</v>
       </c>
-      <c r="C20">
-        <f t="shared" ref="C20:E20" si="1">AVERAGE(C18:C19)</f>
+      <c r="C19">
+        <f t="shared" ref="C19:E19" si="1">AVERAGE(C17:C18)</f>
         <v>30</v>
       </c>
-      <c r="D20">
+      <c r="D19">
         <f t="shared" si="1"/>
         <v>26.5</v>
       </c>
-      <c r="E20">
+      <c r="E19">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="16">
+        <v>52</v>
+      </c>
+      <c r="C20" s="16">
+        <v>69</v>
+      </c>
+      <c r="D20" s="16">
+        <v>63</v>
+      </c>
+      <c r="E20" s="16">
+        <v>75</v>
+      </c>
+      <c r="F20" s="16">
+        <f>SUM(B20:E20)</f>
+        <v>259</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="24"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="16">
+        <v>41</v>
+      </c>
+      <c r="C24" s="16">
+        <v>77</v>
+      </c>
+      <c r="D24" s="16">
+        <v>16</v>
+      </c>
+      <c r="E24" s="16">
+        <v>21</v>
+      </c>
+      <c r="F24" s="16">
+        <f>SUM(B24:E24)</f>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="17">
-        <v>52</v>
-      </c>
-      <c r="C21" s="17">
-        <v>69</v>
-      </c>
-      <c r="D21" s="17">
-        <v>63</v>
-      </c>
-      <c r="E21" s="17">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="9"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="17">
-        <v>41</v>
-      </c>
-      <c r="C25" s="17">
-        <v>77</v>
-      </c>
-      <c r="D25" s="17">
-        <v>16</v>
-      </c>
-      <c r="E25" s="17">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="9"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="13" t="s">
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="21"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="13">
+      <c r="B28" s="13">
         <v>35</v>
       </c>
-      <c r="C29" s="13">
-        <f>C30+1.5</f>
+      <c r="C28" s="13">
+        <f>C29+1.5</f>
         <v>182.5</v>
       </c>
-      <c r="D29" s="13">
-        <f t="shared" ref="D29:E29" si="2">D30+1.5</f>
+      <c r="D28" s="13">
+        <f t="shared" ref="D28:E28" si="2">D29+1.5</f>
         <v>36.5</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E28" s="13">
         <f t="shared" si="2"/>
         <v>56.5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="14" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B29" s="14">
         <v>33</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C29" s="14">
         <v>181</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D29" s="14">
         <v>35</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E29" s="14">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B31">
-        <f>AVERAGE(B29:B30)</f>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <f>AVERAGE(B28:B29)</f>
         <v>34</v>
       </c>
-      <c r="C31">
-        <f t="shared" ref="C31:E31" si="3">AVERAGE(C29:C30)</f>
+      <c r="C30">
+        <f t="shared" ref="C30:E30" si="3">AVERAGE(C28:C29)</f>
         <v>181.75</v>
       </c>
-      <c r="D31">
+      <c r="D30">
         <f t="shared" si="3"/>
         <v>35.75</v>
       </c>
-      <c r="E31">
+      <c r="E30">
         <f t="shared" si="3"/>
         <v>55.75</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="17">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="16">
         <v>56</v>
       </c>
-      <c r="C32" s="17">
+      <c r="C31" s="16">
         <v>216</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D31" s="16">
         <v>77</v>
       </c>
-      <c r="E32" s="17">
+      <c r="E31" s="16">
         <v>102</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>28</v>
-      </c>
-      <c r="B44" s="16">
-        <f>B14/B21</f>
-        <v>1.0961538461538463</v>
-      </c>
-      <c r="C44" s="16">
-        <f>C14/C21</f>
-        <v>3.6956521739130435</v>
-      </c>
-      <c r="D44" s="16">
-        <f>D14/D21</f>
-        <v>1.3015873015873016</v>
-      </c>
-      <c r="E44" s="16">
-        <f>E14/E21</f>
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="F31" s="16">
+        <f>SUM(B31:E31)</f>
+        <v>451</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="19"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="12">
-        <f>B13/B20</f>
-        <v>1.4761904761904763</v>
-      </c>
-      <c r="C45" s="12">
-        <f>C13/C20</f>
-        <v>6.15</v>
-      </c>
-      <c r="D45" s="12">
-        <f>D13/D20</f>
-        <v>1.6226415094339623</v>
-      </c>
-      <c r="E45" s="12">
-        <f>E13/E20</f>
-        <v>2.193548387096774</v>
+      <c r="B34" s="16">
+        <v>27</v>
+      </c>
+      <c r="C34" s="16">
+        <v>35</v>
+      </c>
+      <c r="D34" s="16">
+        <v>19</v>
+      </c>
+      <c r="E34" s="16">
+        <v>17</v>
+      </c>
+      <c r="F34" s="16">
+        <f>SUM(B34:E34)</f>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3213,24 +3239,24 @@
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18" t="s">
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
☑️ Opmaak frontend verfijnen
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nielsonderbeke/Desktop/3MCT-WAD/research-project/research-project-3mct/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D0EB19-719A-8740-AB65-EFE4188449CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4848D962-DF05-764A-BD2F-A849017FEB5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="53760" yWindow="500" windowWidth="19200" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,15 +109,6 @@
     <t>Frontend</t>
   </si>
   <si>
-    <t>4,18 kB</t>
-  </si>
-  <si>
-    <t>51,51 kB</t>
-  </si>
-  <si>
-    <t>6,12 kB</t>
-  </si>
-  <si>
     <t>user 1</t>
   </si>
   <si>
@@ -128,9 +119,6 @@
   </si>
   <si>
     <t>post 12</t>
-  </si>
-  <si>
-    <t>2,47 kB</t>
   </si>
   <si>
     <t>mount tot inladen data</t>
@@ -146,6 +134,18 @@
   </si>
   <si>
     <t>total ms</t>
+  </si>
+  <si>
+    <t>53.39 kB</t>
+  </si>
+  <si>
+    <t>5.17 kB</t>
+  </si>
+  <si>
+    <t>7.3 kB</t>
+  </si>
+  <si>
+    <t>2.69 kB</t>
   </si>
 </sst>
 </file>
@@ -317,9 +317,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -329,6 +326,9 @@
     <xf numFmtId="164" fontId="2" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2482,24 +2482,24 @@
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17" t="s">
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17" t="s">
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
       <c r="N4" s="11"/>
       <c r="O4" s="11" t="s">
         <v>11</v>
@@ -2730,7 +2730,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2746,19 +2746,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2775,16 +2775,16 @@
         <v>17</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2884,7 +2884,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B13" s="16">
         <v>57</v>
@@ -2904,13 +2904,13 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="26"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="25"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
@@ -2945,7 +2945,7 @@
       <c r="E18" s="14">
         <v>30</v>
       </c>
-      <c r="I18" s="22"/>
+      <c r="I18" s="21"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B19">
@@ -2967,7 +2967,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B20" s="16">
         <v>52</v>
@@ -2987,17 +2987,17 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="24"/>
+      <c r="A23" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="23"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B24" s="16">
         <v>41</v>
@@ -3017,13 +3017,13 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="21"/>
+      <c r="A27" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="20"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
@@ -3082,7 +3082,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B31" s="16">
         <v>56</v>
@@ -3102,17 +3102,17 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="19"/>
+      <c r="A33" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="18"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B34" s="16">
         <v>27</v>
@@ -3239,24 +3239,24 @@
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17" t="s">
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17" t="s">
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
💭 Define result criteria
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nielsonderbeke/Desktop/3MCT-WAD/research-project/research-project-3mct/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4848D962-DF05-764A-BD2F-A849017FEB5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CF5576-2B6C-7E4A-8359-A4167D573A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53760" yWindow="500" windowWidth="19200" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34560" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetingen" sheetId="4" r:id="rId1"/>
     <sheet name="Meetingen frontend &amp; backend" sheetId="5" r:id="rId2"/>
-    <sheet name="n sneller data grote" sheetId="2" r:id="rId3"/>
-    <sheet name="n sneller nesting" sheetId="3" r:id="rId4"/>
+    <sheet name="Dev experience" sheetId="6" r:id="rId3"/>
+    <sheet name="n sneller data grote" sheetId="2" r:id="rId4"/>
+    <sheet name="n sneller nesting" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="51">
   <si>
     <t>Caching meetresultaten</t>
   </si>
@@ -127,12 +128,6 @@
     <t>Apollo client cache</t>
   </si>
   <si>
-    <t>Apollo client - persisted queries - without cdn - own server memory cache</t>
-  </si>
-  <si>
-    <t>Apollo client - persisted queries - without cdn - own server memory cache - HTTP CACHE</t>
-  </si>
-  <si>
     <t>total ms</t>
   </si>
   <si>
@@ -146,6 +141,69 @@
   </si>
   <si>
     <t>2.69 kB</t>
+  </si>
+  <si>
+    <t>graphCDN</t>
+  </si>
+  <si>
+    <t>Strategies</t>
+  </si>
+  <si>
+    <t>avg ms</t>
+  </si>
+  <si>
+    <t>Apollo Persisted Queries</t>
+  </si>
+  <si>
+    <t>Apollo Persisted Queries with HTTP Caching</t>
+  </si>
+  <si>
+    <t>Total ms mount component till data loaded (lower=better)</t>
+  </si>
+  <si>
+    <t>AVG ms mount component till data loaded (lower=better)</t>
+  </si>
+  <si>
+    <t>Dev experience</t>
+  </si>
+  <si>
+    <t>Cons</t>
+  </si>
+  <si>
+    <t>Pros</t>
+  </si>
+  <si>
+    <t>Costs</t>
+  </si>
+  <si>
+    <t>Easy to setup (1-10)</t>
+  </si>
+  <si>
+    <t>Caching per field, Fast to setup, Highly customizable, micro services, dockerizeable</t>
+  </si>
+  <si>
+    <t>Knowledge about Redis required, Only resolver result caching (not full response), Stale data own responsibility</t>
+  </si>
+  <si>
+    <t>free</t>
+  </si>
+  <si>
+    <t>free under 5M requests per month https://graphcdn.io/pricing</t>
+  </si>
+  <si>
+    <t>Fast, Auto invalidation (update), 4 cache options, Super easy with React, Great Dev Tools in Chrome, out of the box error &amp; loading states</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Easy to setup with client &amp; server lib, cachable in browser &amp; cdn </t>
+  </si>
+  <si>
+    <t>Invalidation? , How to implement with mutations?, Extra traffic when not know by server</t>
+  </si>
+  <si>
+    <t>Super easy to get up and running, distributed, automatic analytics, highly configurable</t>
+  </si>
+  <si>
+    <t>Sometimes buggy site?, Costs</t>
   </si>
 </sst>
 </file>
@@ -202,7 +260,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -281,6 +339,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -295,7 +359,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -326,8 +390,13 @@
     <xf numFmtId="164" fontId="2" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="14" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -353,6 +422,618 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-BE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Meetingen frontend &amp; backend'!$M$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total ms mount component till data loaded (lower=better)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Meetingen frontend &amp; backend'!$L$5:$L$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>No Cache</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Redis Cache</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Apollo client cache</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apollo Persisted Queries</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Apollo Persisted Queries with HTTP Caching</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>graphCDN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Meetingen frontend &amp; backend'!$M$5:$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>502</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>259</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>451</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>290</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D24E-254D-BABC-0A1679C6940E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1691748928"/>
+        <c:axId val="1691750576"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1691748928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-BE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1691750576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1691750576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-BE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1691748928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-BE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-BE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Meetingen frontend &amp; backend'!$N$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AVG ms mount component till data loaded (lower=better)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Meetingen frontend &amp; backend'!$L$5:$L$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>No Cache</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Redis Cache</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Apollo client cache</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apollo Persisted Queries</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Apollo Persisted Queries with HTTP Caching</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>graphCDN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Meetingen frontend &amp; backend'!$N$5:$N$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>125.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>112.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>72.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F42B-EC40-9898-59A7B5F0F165}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1888506272"/>
+        <c:axId val="1888507952"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1888506272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-BE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1888507952"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1888507952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-BE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1888506272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-BE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -666,7 +1347,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -1059,6 +1740,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2065,7 +2826,1090 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>218017</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>137583</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>645583</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>23283</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F3C81F6-1AEF-2645-A75A-577472BD7134}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>88901</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>165101</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03666CB4-A861-154B-9324-27BA65C22DBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2106,7 +3950,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2482,24 +4326,24 @@
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26" t="s">
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26" t="s">
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
       <c r="N4" s="11"/>
       <c r="O4" s="11" t="s">
         <v>11</v>
@@ -2727,24 +4571,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A49B06-8EDD-4703-89E7-71FF6DEBDE86}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>21</v>
       </c>
@@ -2758,10 +4604,13 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2770,24 +4619,33 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="E4" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="L4" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -2803,8 +4661,20 @@
       <c r="E5" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="L5" s="7" t="str">
+        <f>A9</f>
+        <v>No Cache</v>
+      </c>
+      <c r="M5">
+        <f>F13</f>
+        <v>502</v>
+      </c>
+      <c r="N5">
+        <f>G13</f>
+        <v>125.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -2820,8 +4690,48 @@
       <c r="E6" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="L6" s="24" t="str">
+        <f>A16</f>
+        <v>Redis Cache</v>
+      </c>
+      <c r="M6">
+        <f>F20</f>
+        <v>259</v>
+      </c>
+      <c r="N6">
+        <f>G20</f>
+        <v>64.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L7" s="22" t="str">
+        <f>A23</f>
+        <v>Apollo client cache</v>
+      </c>
+      <c r="M7">
+        <f>F24</f>
+        <v>155</v>
+      </c>
+      <c r="N7">
+        <f>G24</f>
+        <v>38.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L8" s="19" t="str">
+        <f>A27</f>
+        <v>Apollo Persisted Queries</v>
+      </c>
+      <c r="M8">
+        <f>F31</f>
+        <v>451</v>
+      </c>
+      <c r="N8">
+        <f>G31</f>
+        <v>112.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>3</v>
       </c>
@@ -2829,8 +4739,20 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="L9" s="17" t="str">
+        <f>A33</f>
+        <v>Apollo Persisted Queries with HTTP Caching</v>
+      </c>
+      <c r="M9">
+        <f>F34</f>
+        <v>98</v>
+      </c>
+      <c r="N9">
+        <f>G34</f>
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>18</v>
       </c>
@@ -2846,8 +4768,20 @@
       <c r="E10" s="13">
         <v>69</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="L10" s="26" t="str">
+        <f>A36</f>
+        <v>graphCDN</v>
+      </c>
+      <c r="M10">
+        <f>F38</f>
+        <v>290</v>
+      </c>
+      <c r="N10">
+        <f>G38</f>
+        <v>72.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>1</v>
       </c>
@@ -2864,7 +4798,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B12">
         <f>AVERAGE(B10:B11)</f>
         <v>31</v>
@@ -2882,7 +4816,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>23</v>
       </c>
@@ -2902,8 +4836,12 @@
         <f>SUM(B13:E13)</f>
         <v>502</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="16">
+        <f>AVERAGE(B13:E13)</f>
+        <v>125.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="s">
         <v>2</v>
       </c>
@@ -2985,6 +4923,10 @@
         <f>SUM(B20:E20)</f>
         <v>259</v>
       </c>
+      <c r="G20" s="16">
+        <f>AVERAGE(B20:E20)</f>
+        <v>64.75</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
@@ -3015,10 +4957,14 @@
         <f>SUM(B24:E24)</f>
         <v>155</v>
       </c>
+      <c r="G24" s="16">
+        <f>AVERAGE(B24:E24)</f>
+        <v>38.75</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
@@ -3100,17 +5046,21 @@
         <f>SUM(B31:E31)</f>
         <v>451</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31" s="16">
+        <f>AVERAGE(B31:E31)</f>
+        <v>112.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
       <c r="E33" s="18"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
         <v>23</v>
       </c>
@@ -3129,6 +5079,173 @@
       <c r="F34" s="16">
         <f>SUM(B34:E34)</f>
         <v>98</v>
+      </c>
+      <c r="G34" s="16">
+        <f>AVERAGE(B34:E34)</f>
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="27"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="13">
+        <v>24</v>
+      </c>
+      <c r="C37" s="13">
+        <v>45</v>
+      </c>
+      <c r="D37" s="13">
+        <v>25</v>
+      </c>
+      <c r="E37" s="13">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="16">
+        <v>55</v>
+      </c>
+      <c r="C38" s="16">
+        <v>87</v>
+      </c>
+      <c r="D38" s="16">
+        <v>66</v>
+      </c>
+      <c r="E38" s="16">
+        <v>82</v>
+      </c>
+      <c r="F38" s="16">
+        <f>SUM(B38:E38)</f>
+        <v>290</v>
+      </c>
+      <c r="G38" s="16">
+        <f>AVERAGE(B38:E38)</f>
+        <v>72.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A5B55D-CB8B-7247-A828-793F51A9D090}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3136,7 +5253,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C6A869-BC33-4152-8637-9185423EF725}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3196,7 +5313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53CE187-2852-45DF-91A3-78FFA61430C8}">
   <dimension ref="A1:R30"/>
   <sheetViews>
@@ -3239,24 +5356,24 @@
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26" t="s">
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26" t="s">
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6" t="s">
         <v>11</v>

</xml_diff>